<commit_message>
SO TCs updated with SO creation and Line addition through SOAPI and added all product types.
</commit_message>
<xml_diff>
--- a/templates/SOAPI.xlsx
+++ b/templates/SOAPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Automation_1Updated\rsqasampleproj\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF406D7-C672-46E4-8C59-F0AA6758D0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648276C8-3755-423F-AB9C-82672A0DD56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{4577C28F-78BB-496A-9D91-BBA99229E5AB}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{4577C28F-78BB-496A-9D91-BBA99229E5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Header" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="56">
   <si>
     <t>API Mode</t>
   </si>
@@ -195,6 +195,21 @@
   </si>
   <si>
     <t>Change Line</t>
+  </si>
+  <si>
+    <t>a5N0W000001HsIU</t>
+  </si>
+  <si>
+    <t>a5N0W000001HpIt</t>
+  </si>
+  <si>
+    <t>a5N6T0000011eQy</t>
+  </si>
+  <si>
+    <t>a5N0W000001I396</t>
+  </si>
+  <si>
+    <t>a5N0W000001I39B</t>
   </si>
 </sst>
 </file>
@@ -564,7 +579,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,10 +838,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07220FA-1468-4709-AC78-191014F6B4FF}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +898,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -898,18 +913,158 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2">
+        <v>200</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
         <v>100</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>80</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1201,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3FC22D3-7105-47EB-9F93-CBB5CCC1A1D8}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>

</xml_diff>